<commit_message>
Add provenance info for collections
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/Photocatalsis_LIKAT_template043.xlsx
+++ b/inbox-excel-vocabs/Photocatalsis_LIKAT_template043.xlsx
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="501">
   <si>
     <t xml:space="preserve">Created by </t>
   </si>
@@ -1639,37 +1639,19 @@
     <t>Members by Pref. Label</t>
   </si>
   <si>
-    <t>ex:photo/general-terms-coll</t>
-  </si>
-  <si>
-    <t>ex:photo/photocatalytic-co2-reduction-coll</t>
-  </si>
-  <si>
     <t>Reactor design, Synthesis of photocatalyst, Characterization of photocatalysts,  Evaluation of performance</t>
   </si>
   <si>
-    <t>ex:photo/reactor-design-coll</t>
-  </si>
-  <si>
     <t>Reactor design</t>
   </si>
   <si>
     <t>Operation temperature, Operation pressure, Operation mode, Reaction chamber, Light sources, Product identification method, Gas flows</t>
   </si>
   <si>
-    <t>ex:photo/synthesis-of-photocatalysts-coll</t>
-  </si>
-  <si>
     <t>Literature research, Chemical substances used for synthesis, Synthesis steps</t>
   </si>
   <si>
-    <t>ex:photo/characterization-of-photocatalysts-coll</t>
-  </si>
-  <si>
     <t>Gas chromatography, X-ray fluorescence, Electron energy loss spectroscopy, Raman Spectroscopy, Atomic force microscopy, Differential scanning calorimetry, Thermogravimetric analysis, Nuclear magnetic resonance spectroscopy, Photoluminescence, Scanning electron microscopy, X-ray photoelectron spectroscopy, X-ray diffraction, Transmission electron microscopy, Ultraviolet-visible spectroscopy, Fourier transform infrared spectroscopy, Liquid chromatography, Mass spectroscopy</t>
-  </si>
-  <si>
-    <t>ex:photo/evaluation-of-performance-coll</t>
   </si>
   <si>
     <t>Concentration of reactants, Purity of reactants, Operation mode, Light source, Duration of experiment, Irradiation timel Sampling intervals, Form of a catalyst</t>
@@ -2060,102 +2042,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFD9EAD3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB47CFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB47CFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB47CFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB47CFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB47CFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB47CFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB47CFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2361,6 +2247,102 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD9EAD3"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB47CFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB47CFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB47CFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB47CFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB47CFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB47CFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB47CFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2454,19 +2436,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:J156" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:J156" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A2:J156"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Concept IRI*" dataDxfId="19" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" name="Preferred Label*" dataDxfId="18"/>
-    <tableColumn id="3" name="Preferred Label Lang code" dataDxfId="17"/>
-    <tableColumn id="4" name="Definition*" dataDxfId="16"/>
-    <tableColumn id="5" name="Definition Language Code" dataDxfId="15"/>
-    <tableColumn id="6" name="Alternate Label" dataDxfId="14"/>
-    <tableColumn id="7" name="Children URI" dataDxfId="13"/>
-    <tableColumn id="8" name="Provenance" dataDxfId="12"/>
-    <tableColumn id="9" name="Source Vocab URI" dataDxfId="11"/>
-    <tableColumn id="10" name="Children by Pref. Label" dataDxfId="10"/>
+    <tableColumn id="1" name="Concept IRI*" dataDxfId="10" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" name="Preferred Label*" dataDxfId="9"/>
+    <tableColumn id="3" name="Preferred Label Lang code" dataDxfId="8"/>
+    <tableColumn id="4" name="Definition*" dataDxfId="7"/>
+    <tableColumn id="5" name="Definition Language Code" dataDxfId="6"/>
+    <tableColumn id="6" name="Alternate Label" dataDxfId="5"/>
+    <tableColumn id="7" name="Children URI" dataDxfId="4"/>
+    <tableColumn id="8" name="Provenance" dataDxfId="3"/>
+    <tableColumn id="9" name="Source Vocab URI" dataDxfId="2"/>
+    <tableColumn id="10" name="Children by Pref. Label" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4073,42 +4055,42 @@
     <mergeCell ref="H14:J14"/>
   </mergeCells>
   <conditionalFormatting sqref="H17:J18 K1:K8 K17:K28 H3:J7 H10:J10 H8 K10:K15 H13:J13 H14 A18:G18 A15:J15 A19:J28 A10:G14 A2:G8 A1:J1 A9:K9">
-    <cfRule type="containsBlanks" dxfId="9" priority="13">
+    <cfRule type="containsBlanks" dxfId="21" priority="13">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:J4 A2:G2">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="14">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:B17">
-    <cfRule type="containsBlanks" dxfId="7" priority="10">
+    <cfRule type="containsBlanks" dxfId="19" priority="10">
       <formula>LEN(TRIM(A17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="18" priority="7">
       <formula>LEN(TRIM(H2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16 H16:K16">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
+    <cfRule type="containsBlanks" dxfId="17" priority="5">
       <formula>LEN(TRIM(C16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:B16">
-    <cfRule type="containsBlanks" dxfId="4" priority="4">
+    <cfRule type="containsBlanks" dxfId="16" priority="4">
       <formula>LEN(TRIM(A16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
+    <cfRule type="containsBlanks" dxfId="15" priority="3">
       <formula>LEN(TRIM(C17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J12">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="14" priority="1">
       <formula>LEN(TRIM(H12))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6989,7 +6971,7 @@
     <mergeCell ref="B158:I158"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:J160">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="13" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10161,7 +10143,7 @@
   <dimension ref="A1:J541"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11025,11 +11007,11 @@
       <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A37" s="38"/>
-      <c r="B37" s="19" t="s">
+      <c r="A37" s="17"/>
+      <c r="B37" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="19" t="s">
         <v>69</v>
       </c>
       <c r="D37" s="13" t="s">
@@ -11049,11 +11031,11 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A38" s="38"/>
-      <c r="B38" s="19" t="s">
+      <c r="A38" s="17"/>
+      <c r="B38" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="19" t="s">
         <v>69</v>
       </c>
       <c r="D38" s="13" t="s">
@@ -11071,11 +11053,11 @@
       <c r="J38" s="13"/>
     </row>
     <row r="39" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A39" s="38"/>
-      <c r="B39" s="19" t="s">
+      <c r="A39" s="17"/>
+      <c r="B39" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="C39" s="39" t="s">
+      <c r="C39" s="19" t="s">
         <v>69</v>
       </c>
       <c r="D39" s="13" t="s">
@@ -23608,7 +23590,7 @@
   <dimension ref="A1:F200"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23654,9 +23636,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>491</v>
-      </c>
+      <c r="A3" s="29"/>
       <c r="B3" s="12" t="s">
         <v>74</v>
       </c>
@@ -23664,15 +23644,15 @@
         <v>75</v>
       </c>
       <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
+      <c r="E3" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="F3" s="27" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
-        <v>492</v>
-      </c>
+      <c r="A4" s="29"/>
       <c r="B4" s="27" t="s">
         <v>28</v>
       </c>
@@ -23680,30 +23660,31 @@
         <v>70</v>
       </c>
       <c r="D4" s="27"/>
+      <c r="E4" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="F4" s="27" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
-        <v>494</v>
-      </c>
+      <c r="A5" s="29"/>
       <c r="B5" s="27" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>146</v>
       </c>
       <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
+      <c r="E5" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="F5" s="27" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
-        <v>497</v>
-      </c>
+      <c r="A6" s="29"/>
       <c r="B6" s="27" t="s">
         <v>257</v>
       </c>
@@ -23711,15 +23692,15 @@
         <v>258</v>
       </c>
       <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
+      <c r="E6" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="F6" s="27" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
-        <v>499</v>
-      </c>
+      <c r="A7" s="29"/>
       <c r="B7" s="27" t="s">
         <v>306</v>
       </c>
@@ -23727,15 +23708,15 @@
         <v>307</v>
       </c>
       <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
+      <c r="E7" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="F7" s="27" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
-        <v>501</v>
-      </c>
+      <c r="A8" s="29"/>
       <c r="B8" s="27" t="s">
         <v>365</v>
       </c>
@@ -23743,9 +23724,11 @@
         <v>366</v>
       </c>
       <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="E8" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="F8" s="27" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -25120,18 +25103,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>